<commit_message>
actualizacion de table y impresoras.xlsx
</commit_message>
<xml_diff>
--- a/src/Impresoras.xlsx
+++ b/src/Impresoras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imeza\Documents\proyecto stock\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCCFEFA-695E-4D71-BCC6-1DAF596740DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFD67D0-4B2C-4D26-9E61-3D7BA45B00B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="1290" windowWidth="21600" windowHeight="11385" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTALACION DE EQUIPOS  - MPRES" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,9 @@
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filtro 1" guid="{C36CE274-4119-4705-869C-657D6C8B4A32}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filtro 2" guid="{39C1E986-E83B-4782-B6F1-6C45A37C89DD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filtro 3" guid="{5B86111C-FE5F-4030-B282-2A29BD6AACF1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filtro 2" guid="{39C1E986-E83B-4782-B6F1-6C45A37C89DD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filtro 1" guid="{C36CE274-4119-4705-869C-657D6C8B4A32}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -2342,9 +2342,9 @@
   </sheetPr>
   <dimension ref="A1:EJ992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -22828,30 +22828,18 @@
   </sheetData>
   <autoFilter ref="A1:K109" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{5B86111C-FE5F-4030-B282-2A29BD6AACF1}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C36CE274-4119-4705-869C-657D6C8B4A32}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="D1:D329" xr:uid="{0EB2D9EB-2A4D-41A5-990C-ABDE47CD3D84}">
-        <filterColumn colId="0">
-          <filters>
-            <filter val="BROTHER 3150 - (Color)"/>
-            <filter val="HP  432 (Nueva)"/>
-            <filter val="HP432 (Nueva)"/>
-            <filter val="Konica Minolta  - bizhub C308 - Color  - A3"/>
-            <filter val="Konica Minolta - bizhub 554 - Negra A3"/>
-            <filter val="Konica Minolta - bizhub C368 - color"/>
-            <filter val="Konica Minolta Bizhub C558"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
+      <autoFilter ref="A1:H108" xr:uid="{74D68FA5-30C0-4E4A-91B0-9EE9C980C620}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="579181608"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1382544901"/>
         </ext>
       </extLst>
     </customSheetView>
     <customSheetView guid="{39C1E986-E83B-4782-B6F1-6C45A37C89DD}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="D1:D329" xr:uid="{2C037058-0F13-4948-8B4A-911F87F256F3}">
+      <autoFilter ref="D1:D329" xr:uid="{1AD0928D-BCFA-4556-AE37-CAB841DAAAA5}">
         <filterColumn colId="0">
           <filters>
             <filter val="BROTHER 3150 - (Color)"/>
@@ -22875,12 +22863,24 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{C36CE274-4119-4705-869C-657D6C8B4A32}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{5B86111C-FE5F-4030-B282-2A29BD6AACF1}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:H108" xr:uid="{B5095417-0400-4246-B33C-71161CC3B1F7}"/>
+      <autoFilter ref="D1:D329" xr:uid="{7B802DD8-3256-45C0-B032-18AD6644549D}">
+        <filterColumn colId="0">
+          <filters>
+            <filter val="BROTHER 3150 - (Color)"/>
+            <filter val="HP  432 (Nueva)"/>
+            <filter val="HP432 (Nueva)"/>
+            <filter val="Konica Minolta  - bizhub C308 - Color  - A3"/>
+            <filter val="Konica Minolta - bizhub 554 - Negra A3"/>
+            <filter val="Konica Minolta - bizhub C368 - color"/>
+            <filter val="Konica Minolta Bizhub C558"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1382544901"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="579181608"/>
         </ext>
       </extLst>
     </customSheetView>

</xml_diff>